<commit_message>
add over all analysis
</commit_message>
<xml_diff>
--- a/src/main/resources/Mappe1.xlsx
+++ b/src/main/resources/Mappe1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="28515" windowHeight="12585" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="28515" windowHeight="12585" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -16,12 +16,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>test</t>
   </si>
   <si>
     <t>xxxxxxxxxx</t>
+  </si>
+  <si>
+    <t>Test Long String</t>
   </si>
 </sst>
 </file>
@@ -387,7 +390,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
@@ -405,12 +408,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="4" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>